<commit_message>
Fixed several weights that wre off
</commit_message>
<xml_diff>
--- a/Data/gill_net_fish_data_2021.xlsx
+++ b/Data/gill_net_fish_data_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\CU\Data\LT age estimation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514E4015-A9F2-4267-AB66-9AF5BBBDFBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{36249BF2-CB3D-4E20-93A0-8EA51D5EA94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0BD1DB14-2411-4060-B255-42B4EDDB943F}"/>
+    <workbookView xWindow="-19320" yWindow="720" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{0BD1DB14-2411-4060-B255-42B4EDDB943F}"/>
   </bookViews>
   <sheets>
     <sheet name="gill_net_fish_data_2021" sheetId="1" r:id="rId1"/>
@@ -1003,44 +1003,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2DCC3B-FF32-48C6-AF2B-19EE610F9AE8}">
   <dimension ref="A1:AC105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD40" sqref="AC39:AD40"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T98" sqref="T97:T98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="54.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="54.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.21875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" style="1"/>
-    <col min="20" max="20" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.88671875" style="1"/>
-    <col min="23" max="23" width="8.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.77734375" style="1" customWidth="1"/>
-    <col min="25" max="25" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="166.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="8.88671875" style="1"/>
+    <col min="15" max="15" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" style="1"/>
+    <col min="20" max="20" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" style="1"/>
+    <col min="23" max="23" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.7109375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="166.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44321</v>
       </c>
@@ -1204,7 +1204,7 @@
       </c>
       <c r="AC2" s="10"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44323</v>
       </c>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="AC3" s="24"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44323</v>
       </c>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="AC4" s="20"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44329</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44319</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44321</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>44330</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>44330</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>44328</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>44321</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>44321</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>44328</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>44321</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>44323</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>44329</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>44323</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>44330</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>44321</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>44323</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>44323</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>44329</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>44323</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>44323</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>44323</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>44330</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>44329</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>44323</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>44323</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>44321</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>215</v>
       </c>
       <c r="T30" s="1">
-        <v>194</v>
+        <v>940</v>
       </c>
       <c r="U30" s="1" t="s">
         <v>26</v>
@@ -3188,7 +3188,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>44323</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>44329</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>44323</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>44330</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>44321</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>44323</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>44323</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>44330</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>44321</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>44330</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>44319</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>44323</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>44329</v>
       </c>
@@ -4105,7 +4105,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14">
         <v>44329</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="14">
         <v>44323</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14">
         <v>44330</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14">
         <v>44321</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:27" s="10" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:27" s="10" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>44322</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:27" s="10" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:27" s="10" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>44322</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:27" s="10" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:27" s="10" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <v>44322</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:27" s="10" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:27" s="10" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <v>44322</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:27" s="10" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:27" s="10" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>44322</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:27" s="10" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:27" s="10" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
         <v>44322</v>
       </c>
@@ -4830,7 +4830,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
         <v>44328</v>
       </c>
@@ -4898,7 +4898,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="19">
         <v>44322</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="19">
         <v>44322</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="19">
         <v>44329</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="19">
         <v>44322</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="19">
         <v>44322</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="19">
         <v>44322</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="19">
         <v>44328</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>44322</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>44320</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>44327</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>44327</v>
       </c>
@@ -5664,7 +5664,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>44319</v>
       </c>
@@ -5729,7 +5729,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>44328</v>
       </c>
@@ -5800,7 +5800,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>44320</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>44329</v>
       </c>
@@ -5936,7 +5936,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>44328</v>
       </c>
@@ -6007,7 +6007,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>44319</v>
       </c>
@@ -6081,7 +6081,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <v>44320</v>
       </c>
@@ -6146,7 +6146,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>44322</v>
       </c>
@@ -6220,7 +6220,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="74" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="9">
         <v>44322</v>
       </c>
@@ -6291,7 +6291,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
         <v>44319</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <v>44322</v>
       </c>
@@ -6433,7 +6433,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
         <v>44319</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <v>44328</v>
       </c>
@@ -6575,7 +6575,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
         <v>44328</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>44329</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>44327</v>
       </c>
@@ -6785,7 +6785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>44319</v>
       </c>
@@ -6865,7 +6865,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>44320</v>
       </c>
@@ -6924,7 +6924,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>44329</v>
       </c>
@@ -6995,7 +6995,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>44328</v>
       </c>
@@ -7066,7 +7066,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>44327</v>
       </c>
@@ -7137,7 +7137,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>44319</v>
       </c>
@@ -7196,7 +7196,7 @@
         <v>220</v>
       </c>
       <c r="T87" s="1">
-        <v>450</v>
+        <v>1150</v>
       </c>
       <c r="U87" s="1" t="s">
         <v>26</v>
@@ -7208,7 +7208,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>44322</v>
       </c>
@@ -7279,7 +7279,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14">
         <v>44327</v>
       </c>
@@ -7350,7 +7350,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="14">
         <v>44327</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="14">
         <v>44327</v>
       </c>
@@ -7490,7 +7490,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="14">
         <v>44327</v>
       </c>
@@ -7564,7 +7564,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="93" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="14">
         <v>44327</v>
       </c>
@@ -7636,7 +7636,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>44322</v>
       </c>
@@ -7704,7 +7704,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>44320</v>
       </c>
@@ -7748,7 +7748,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>44320</v>
       </c>
@@ -7794,7 +7794,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>44322</v>
       </c>
@@ -7862,7 +7862,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>44320</v>
       </c>
@@ -7906,7 +7906,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>44320</v>
       </c>
@@ -7947,7 +7947,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>44329</v>
       </c>
@@ -7996,7 +7996,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>44320</v>
       </c>
@@ -8040,7 +8040,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>44320</v>
       </c>
@@ -8087,7 +8087,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>44320</v>
       </c>
@@ -8107,7 +8107,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>44320</v>
       </c>
@@ -8127,7 +8127,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>44323</v>
       </c>
@@ -8186,16 +8186,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE173A9-0A54-45F5-A9B8-C16B41AB1ABD}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>166</v>
       </c>
@@ -8203,19 +8203,19 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>167</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B3" s="24"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>169</v>
       </c>

</xml_diff>